<commit_message>
main change - update Fixer!
now the greed algo is more stable
our "best" by mistake got a little nerf but now all modes of sorts/unsorts works well

also there is no use anymore to Random funcs to engage the unchoosen calls -> the fixer finds the best elevators to push them that calls
</commit_message>
<xml_diff>
--- a/csv logs and archive/times summerize.xlsx
+++ b/csv logs and archive/times summerize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Desktop\Studies\שנה ב\תכנות מונחה עצמים\Ex1\Ex1\csv logs and archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718D8352-B777-47BB-B2A7-0BBA12F3789C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20005A8D-3089-4F0E-B3E2-71A71AE79DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>log:</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Total waiting time: 1529.0,  average waiting time per call: 15.29,  unCompleted calls,0,  certificate, -238185301</t>
+  </si>
+  <si>
+    <t>Total waiting time: 49011.0,  average waiting time per call: 49.011,  unCompleted calls,0,  certificate, -120713707</t>
+  </si>
+  <si>
+    <t>Total waiting time: 49931.874732,  average waiting time per call: 49.931874732,  unCompleted calls,2,  certificate, -120713699</t>
+  </si>
+  <si>
+    <t>FlexGreedyAlgoSortWithFixer</t>
+  </si>
+  <si>
+    <t>FlexGreedyAlgoNoSortWithFixer</t>
+  </si>
+  <si>
+    <t>Total waiting time: 48702.0,  average waiting time per call: 48.702,  unCompleted calls,0,  certificate, -80037722</t>
+  </si>
+  <si>
+    <t>FlexGreedyAlgoReserveSortWithFixer</t>
+  </si>
+  <si>
+    <t>Total waiting time: 1319.0,  average waiting time per call: 13.19,  unCompleted calls,0,  certificate, -260638911</t>
+  </si>
+  <si>
+    <t>FlexGreedyAlgoReserveSortWithFixer_a</t>
   </si>
 </sst>
 </file>
@@ -421,19 +445,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E12"/>
+  <dimension ref="A3:E16"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86" customWidth="1"/>
+    <col min="1" max="1" width="95" customWidth="1"/>
     <col min="2" max="2" width="8.796875" customWidth="1"/>
     <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="19.296875" customWidth="1"/>
-    <col min="5" max="5" width="26.3984375" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,6 +630,74 @@
         <v>24</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>